<commit_message>
Added a template visualization for the bioscreen
</commit_message>
<xml_diff>
--- a/template_bioscreen.xlsx
+++ b/template_bioscreen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upct-my.sharepoint.com/personal/alberto_garre_upct_es/Documents/MariaZambrano_UPCT-UCO/03_coding/biogrowth4/biogrowth4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_AD4D2F04E46CFB4ACB3E20DEB556E566683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7BA409C-1D11-4CAE-81A9-2238E4478215}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_AD4D2F04E46CFB4ACB3E20DEB556E566683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7669FA1B-C0AB-4496-B1D3-2A777C2A9D69}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28125" yWindow="900" windowWidth="15765" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>condition</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>ST2</t>
+  </si>
+  <si>
+    <t>ST22</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>other to</t>
   </si>
 </sst>
 </file>
@@ -98,6 +107,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A30B8B-4E1A-422E-8D52-1E4BC12BF049}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -422,6 +435,57 @@
         <v>96</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>91</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>